<commit_message>
Feature: update Excel export formats for pre-inscriptions and references
</commit_message>
<xml_diff>
--- a/statics/formato-referencias.xlsx
+++ b/statics/formato-referencias.xlsx
@@ -1,26 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24334"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jossue Irias\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Funval\proyectos\test\sigef\statics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB4E0222-A348-4236-872F-F7FF3C0B74EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54E05E2C-F265-4AB7-BC33-C1E1CEBF0340}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4290" yWindow="4290" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Nombre</t>
   </si>
@@ -43,51 +48,6 @@
     <t>Relación</t>
   </si>
   <si>
-    <t>Daniel Wolke</t>
-  </si>
-  <si>
-    <t>Masculino</t>
-  </si>
-  <si>
-    <t>(+502) 55640719</t>
-  </si>
-  <si>
-    <t>Guatemala</t>
-  </si>
-  <si>
-    <t>Estaca Bosques de San Nicolas</t>
-  </si>
-  <si>
-    <t>Jossue Irias</t>
-  </si>
-  <si>
-    <t>Amigo</t>
-  </si>
-  <si>
-    <t>(+504) 31759499</t>
-  </si>
-  <si>
-    <t>26/09/2025</t>
-  </si>
-  <si>
-    <t>jossue irias</t>
-  </si>
-  <si>
-    <t>(+504) 44444444444</t>
-  </si>
-  <si>
-    <t>Honduras</t>
-  </si>
-  <si>
-    <t>Estaca Tegucigalpa Honduras Villa Olímpica</t>
-  </si>
-  <si>
-    <t>Jossue</t>
-  </si>
-  <si>
-    <t>(+504) 44444555555</t>
-  </si>
-  <si>
     <t>Nombre del referente</t>
   </si>
   <si>
@@ -104,7 +64,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -230,15 +190,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -249,6 +200,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -256,20 +216,6 @@
   <dxfs count="13">
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Aptos Display"/>
-        <family val="2"/>
-        <scheme val="major"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -472,6 +418,20 @@
         <scheme val="major"/>
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Aptos Display"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
@@ -553,18 +513,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B52D9133-2E1E-4F58-A1F4-E6243355C7EF}" name="Tabla2" displayName="Tabla2" ref="B8:K16" totalsRowShown="0" headerRowDxfId="0" dataDxfId="12" tableBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B52D9133-2E1E-4F58-A1F4-E6243355C7EF}" name="Tabla2" displayName="Tabla2" ref="B8:K16" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11" tableBorderDxfId="10">
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{76145434-176B-433D-B1C0-582A200A5CF9}" name="Nombre" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{90253768-D17D-4C26-811C-40BF66B98FC0}" name="Genero" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{AF687271-7984-45E7-A8FB-DF14DE3652FE}" name="Edad" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{4E47F7ED-C13C-40A0-A945-3E9C32D5A021}" name="Número" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{E69B451A-4239-4219-92A5-602044D59BAD}" name="País" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{4DB58426-BFC2-4675-A06E-1F2EC8779380}" name="Estaca o distrito" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{FF29BD52-A890-4B82-9425-3B36B3F957DF}" name="Nombre del referente" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{6F1E2073-236A-4514-8EEA-612006950F15}" name="Relación" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{0C7FC0E5-00AF-46DB-A23D-FCFE9C0ACB8D}" name="Número del referente" dataDxfId="2"/>
-    <tableColumn id="10" xr3:uid="{6AC9306B-8FC5-4705-905B-A425344033B8}" name="Fecha de referencia" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{76145434-176B-433D-B1C0-582A200A5CF9}" name="Nombre" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{90253768-D17D-4C26-811C-40BF66B98FC0}" name="Genero" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{AF687271-7984-45E7-A8FB-DF14DE3652FE}" name="Edad" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{4E47F7ED-C13C-40A0-A945-3E9C32D5A021}" name="Número" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{E69B451A-4239-4219-92A5-602044D59BAD}" name="País" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{4DB58426-BFC2-4675-A06E-1F2EC8779380}" name="Estaca o distrito" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{FF29BD52-A890-4B82-9425-3B36B3F957DF}" name="Nombre del referente" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{6F1E2073-236A-4514-8EEA-612006950F15}" name="Relación" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{0C7FC0E5-00AF-46DB-A23D-FCFE9C0ACB8D}" name="Número del referente" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{6AC9306B-8FC5-4705-905B-A425344033B8}" name="Fecha de referencia" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -894,138 +854,98 @@
   <dimension ref="A7:M16"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.125" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="9.08984375" style="1"/>
-    <col min="2" max="2" width="15.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.125" style="1"/>
+    <col min="2" max="2" width="15.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="37.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.6328125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="27.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.36328125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="9.08984375" style="1"/>
+    <col min="5" max="5" width="18.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="37.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="27.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.375" style="1" customWidth="1"/>
+    <col min="13" max="13" width="9.125" style="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="2:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="4" t="s">
-        <v>23</v>
+    <row r="7" spans="2:12" ht="20.25" customHeight="1">
+      <c r="B7" s="8" t="s">
+        <v>8</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="6"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="10"/>
     </row>
-    <row r="8" spans="2:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B8" s="7" t="s">
+    <row r="8" spans="2:12" ht="20.25" customHeight="1">
+      <c r="B8" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="G8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H8" s="9" t="s">
-        <v>22</v>
+      <c r="H8" s="6" t="s">
+        <v>7</v>
       </c>
-      <c r="I8" s="8" t="s">
+      <c r="I8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="J8" s="8" t="s">
-        <v>24</v>
+      <c r="J8" s="5" t="s">
+        <v>9</v>
       </c>
-      <c r="K8" s="10" t="s">
-        <v>25</v>
+      <c r="K8" s="7" t="s">
+        <v>10</v>
       </c>
       <c r="L8" s="2"/>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B9" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="3">
-        <v>37</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="K9" s="3" t="s">
-        <v>15</v>
-      </c>
+    <row r="9" spans="2:12">
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B10" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="3">
-        <v>24</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K10" s="3" t="s">
-        <v>15</v>
-      </c>
+    <row r="10" spans="2:12">
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:12">
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -1037,7 +957,7 @@
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:12">
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -1049,7 +969,7 @@
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:12">
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -1061,7 +981,7 @@
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:12">
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
@@ -1073,7 +993,7 @@
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:12">
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -1085,7 +1005,7 @@
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:12">
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>

</xml_diff>